<commit_message>
Add new data files and update model outputs
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\SENG438\seng438-a5-aryan-karadia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karad\Desktop\SENG 438\seng438-a5-aryan-karadia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{034E7AF4-6749-4527-A9B1-82DD4F6FC6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAD9F62-B12B-4958-A37A-556BD0A0F497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15885"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>T</t>
   </si>
   <si>
     <t>FC</t>
   </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -894,1405 +885,669 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1.6667000000000001E-2</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>1.6667000000000001E-2</v>
-      </c>
-      <c r="D3">
-        <v>3.3333000000000002E-2</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>28</v>
       </c>
-      <c r="C4">
-        <v>3.3333000000000002E-2</v>
-      </c>
-      <c r="D4">
-        <v>8.3333000000000004E-2</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>8.3333000000000004E-2</v>
-      </c>
-      <c r="D5">
-        <v>0.125</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>0.125</v>
-      </c>
-      <c r="D6">
-        <v>0.20833299999999999</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>0.20833299999999999</v>
-      </c>
-      <c r="D7">
-        <v>0.29166700000000001</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
-      <c r="C8">
-        <v>0.29166700000000001</v>
-      </c>
-      <c r="D8">
-        <v>0.35833300000000001</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>16</v>
       </c>
-      <c r="C9">
-        <v>0.35833300000000001</v>
-      </c>
-      <c r="D9">
-        <v>0.49166700000000002</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10">
-        <v>0.49166700000000002</v>
-      </c>
-      <c r="D10">
-        <v>0.55833299999999997</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>0.55833299999999997</v>
-      </c>
-      <c r="D11">
-        <v>0.64166699999999999</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12">
-        <v>0.64166699999999999</v>
-      </c>
-      <c r="D12">
-        <v>0.7</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>14</v>
       </c>
-      <c r="C13">
-        <v>0.7</v>
-      </c>
-      <c r="D13">
-        <v>0.89166699999999999</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-      <c r="C14">
-        <v>0.89166699999999999</v>
-      </c>
-      <c r="D14">
-        <v>0.95</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15">
-        <v>0.95</v>
-      </c>
-      <c r="D15">
-        <v>0.98333300000000001</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16">
-        <v>0.98333300000000001</v>
-      </c>
-      <c r="D16">
-        <v>1.016667</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>8</v>
       </c>
-      <c r="C17">
-        <v>1.016667</v>
-      </c>
-      <c r="D17">
-        <v>1.0916669999999999</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18">
-        <v>1.0916669999999999</v>
-      </c>
-      <c r="D18">
-        <v>1.2833330000000001</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
-      <c r="C19">
-        <v>1.2833330000000001</v>
-      </c>
-      <c r="D19">
-        <v>1.358333</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
-      <c r="C20">
-        <v>1.358333</v>
-      </c>
-      <c r="D20">
-        <v>1.441667</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
-      <c r="C21">
-        <v>1.441667</v>
-      </c>
-      <c r="D21">
-        <v>1.5916669999999999</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
-      <c r="C22">
-        <v>1.5916669999999999</v>
-      </c>
-      <c r="D22">
-        <v>1.65</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>14</v>
       </c>
-      <c r="C23">
-        <v>1.65</v>
-      </c>
-      <c r="D23">
-        <v>1.8416669999999999</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>9</v>
       </c>
-      <c r="C24">
-        <v>1.8416669999999999</v>
-      </c>
-      <c r="D24">
-        <v>1.925</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
-      <c r="C25">
-        <v>1.925</v>
-      </c>
-      <c r="D25">
-        <v>2.2916669999999999</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>11</v>
       </c>
-      <c r="C26">
-        <v>2.2916669999999999</v>
-      </c>
-      <c r="D26">
-        <v>2.4750000000000001</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>20</v>
       </c>
-      <c r="C27">
-        <v>2.4750000000000001</v>
-      </c>
-      <c r="D27">
-        <v>2.9249999999999998</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>6</v>
       </c>
-      <c r="C28">
-        <v>2.9249999999999998</v>
-      </c>
-      <c r="D28">
-        <v>3</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>3.0333329999999998</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>6</v>
       </c>
-      <c r="C30">
-        <v>3.0333329999999998</v>
-      </c>
-      <c r="D30">
-        <v>3.1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>5</v>
       </c>
-      <c r="C31">
-        <v>3.1</v>
-      </c>
-      <c r="D31">
-        <v>3.1583329999999998</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-      <c r="C32">
-        <v>3.1583329999999998</v>
-      </c>
-      <c r="D32">
-        <v>3.2166670000000002</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33">
-        <v>3.2166670000000002</v>
-      </c>
-      <c r="D33">
-        <v>3.233333</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <v>8</v>
       </c>
-      <c r="C34">
-        <v>3.233333</v>
-      </c>
-      <c r="D34">
-        <v>3.3083330000000002</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
-      <c r="C35">
-        <v>3.3083330000000002</v>
-      </c>
-      <c r="D35">
-        <v>3.3833329999999999</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
-      <c r="C36">
-        <v>3.3833329999999999</v>
-      </c>
-      <c r="D36">
-        <v>3.4083329999999998</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <v>4</v>
       </c>
-      <c r="C37">
-        <v>3.4083329999999998</v>
-      </c>
-      <c r="D37">
-        <v>3.4666670000000002</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38">
-        <v>3.4666670000000002</v>
-      </c>
-      <c r="D38">
-        <v>3.483333</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>14</v>
       </c>
-      <c r="C39">
-        <v>3.483333</v>
-      </c>
-      <c r="D39">
-        <v>3.6749999999999998</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
-      <c r="C40">
-        <v>3.6749999999999998</v>
-      </c>
-      <c r="D40">
-        <v>3.733333</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41">
-        <v>3.733333</v>
-      </c>
-      <c r="D41">
-        <v>3.766667</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
         <v>5</v>
       </c>
-      <c r="C42">
-        <v>3.766667</v>
-      </c>
-      <c r="D42">
-        <v>3.8250000000000002</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="C43">
-        <v>3.8250000000000002</v>
-      </c>
-      <c r="D43">
-        <v>3.85</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
-      <c r="C44">
-        <v>3.85</v>
-      </c>
-      <c r="D44">
-        <v>3.9083329999999998</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <v>11</v>
       </c>
-      <c r="C45">
-        <v>3.9083329999999998</v>
-      </c>
-      <c r="D45">
-        <v>4.0916670000000002</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>6</v>
       </c>
-      <c r="C46">
-        <v>4.0916670000000002</v>
-      </c>
-      <c r="D46">
-        <v>4.1583329999999998</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
-      <c r="C47">
-        <v>4.1583329999999998</v>
-      </c>
-      <c r="D47">
-        <v>4.1583329999999998</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <v>5</v>
       </c>
-      <c r="C48">
-        <v>4.1583329999999998</v>
-      </c>
-      <c r="D48">
-        <v>4.2166670000000002</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
-      <c r="C49">
-        <v>4.2166670000000002</v>
-      </c>
-      <c r="D49">
-        <v>4.25</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
-      <c r="C50">
-        <v>4.25</v>
-      </c>
-      <c r="D50">
-        <v>4.2750000000000004</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
-      <c r="C51">
-        <v>4.2750000000000004</v>
-      </c>
-      <c r="D51">
-        <v>4.2833329999999998</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
-      <c r="C52">
-        <v>4.2833329999999998</v>
-      </c>
-      <c r="D52">
-        <v>4.2833329999999998</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
         <v>3</v>
       </c>
-      <c r="C53">
-        <v>4.2833329999999998</v>
-      </c>
-      <c r="D53">
-        <v>4.3166669999999998</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
-      <c r="C54">
-        <v>4.3166669999999998</v>
-      </c>
-      <c r="D54">
-        <v>4.3166669999999998</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
-      <c r="C55">
-        <v>4.3166669999999998</v>
-      </c>
-      <c r="D55">
-        <v>4.3166669999999998</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
-      <c r="C56">
-        <v>4.3166669999999998</v>
-      </c>
-      <c r="D56">
-        <v>4.3250000000000002</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
         <v>5</v>
       </c>
-      <c r="C57">
-        <v>4.3250000000000002</v>
-      </c>
-      <c r="D57">
-        <v>4.3833330000000004</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
         <v>5</v>
       </c>
-      <c r="C58">
-        <v>4.3833330000000004</v>
-      </c>
-      <c r="D58">
-        <v>4.4416669999999998</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
-      <c r="C59">
-        <v>4.4416669999999998</v>
-      </c>
-      <c r="D59">
-        <v>4.4666670000000002</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
         <v>7</v>
       </c>
-      <c r="C60">
-        <v>4.4666670000000002</v>
-      </c>
-      <c r="D60">
-        <v>4.5416670000000003</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
         <v>6</v>
       </c>
-      <c r="C61">
-        <v>4.5416670000000003</v>
-      </c>
-      <c r="D61">
-        <v>4.608333</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
-      <c r="C62">
-        <v>4.608333</v>
-      </c>
-      <c r="D62">
-        <v>4.6166669999999996</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
         <v>5</v>
       </c>
-      <c r="C63">
-        <v>4.6166669999999996</v>
-      </c>
-      <c r="D63">
-        <v>4.6749999999999998</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
-      <c r="C64">
-        <v>4.6749999999999998</v>
-      </c>
-      <c r="D64">
-        <v>4.6833330000000002</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
-      <c r="C65">
-        <v>4.6833330000000002</v>
-      </c>
-      <c r="D65">
-        <v>4.7166670000000002</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
         <v>6</v>
       </c>
-      <c r="C66">
-        <v>4.7166670000000002</v>
-      </c>
-      <c r="D66">
-        <v>4.7833329999999998</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
         <v>11</v>
       </c>
-      <c r="C67">
-        <v>4.7833329999999998</v>
-      </c>
-      <c r="D67">
-        <v>4.9666670000000002</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
         <v>3</v>
       </c>
-      <c r="C68">
-        <v>4.9666670000000002</v>
-      </c>
-      <c r="D68">
-        <v>5</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
         <v>5</v>
       </c>
-      <c r="C69">
-        <v>5</v>
-      </c>
-      <c r="D69">
-        <v>5.0583330000000002</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
         <v>6</v>
       </c>
-      <c r="C70">
-        <v>5.0583330000000002</v>
-      </c>
-      <c r="D70">
-        <v>5.125</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
         <v>2</v>
       </c>
-      <c r="C71">
-        <v>5.125</v>
-      </c>
-      <c r="D71">
-        <v>5.15</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
-      <c r="C72">
-        <v>5.15</v>
-      </c>
-      <c r="D72">
-        <v>5.15</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
-      <c r="C73">
-        <v>5.15</v>
-      </c>
-      <c r="D73">
-        <v>5.15</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
         <v>1</v>
       </c>
-      <c r="C74">
-        <v>5.15</v>
-      </c>
-      <c r="D74">
-        <v>5.1583329999999998</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75">
         <v>1</v>
       </c>
-      <c r="C75">
-        <v>5.1583329999999998</v>
-      </c>
-      <c r="D75">
-        <v>5.1666670000000003</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
-      <c r="C76">
-        <v>5.1666670000000003</v>
-      </c>
-      <c r="D76">
-        <v>5.1749999999999998</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
-      <c r="C77">
-        <v>5.1749999999999998</v>
-      </c>
-      <c r="D77">
-        <v>5.1749999999999998</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
-      <c r="C78">
-        <v>5.1749999999999998</v>
-      </c>
-      <c r="D78">
-        <v>5.1749999999999998</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
-      <c r="C79">
-        <v>5.1749999999999998</v>
-      </c>
-      <c r="D79">
-        <v>5.1833330000000002</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
-      <c r="C80">
-        <v>5.1833330000000002</v>
-      </c>
-      <c r="D80">
-        <v>5.1833330000000002</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
-      <c r="C81">
-        <v>5.1833330000000002</v>
-      </c>
-      <c r="D81">
-        <v>5.1833330000000002</v>
-      </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
         <v>1</v>
-      </c>
-      <c r="C82">
-        <v>5.1833330000000002</v>
-      </c>
-      <c r="D82">
-        <v>5.1916669999999998</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>